<commit_message>
Edited cld.py module to make it look cleaner
As the title had said. the original script looks like shit, very hard to read. I edited it to make it look easier (at least for me) to read. I also renamed some of the columns referenced in the module to match the output of statsmodel's Tukey test results. And I removed a condition that checks if the format of the p-values are strings.
</commit_message>
<xml_diff>
--- a/alkane, timePoint x Vegetation.xlsx
+++ b/alkane, timePoint x Vegetation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F592254-24F4-48BA-BC1B-085113894BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E63AB6-DE3C-4D2B-9FBF-C1782EE6E607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,13 +58,13 @@
     <t>6 x Shrub</t>
   </si>
   <si>
-    <t>pval</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>p-adj</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,16 +486,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>

</xml_diff>